<commit_message>
my latest chat app
</commit_message>
<xml_diff>
--- a/kubernetes cmd/kubernetes_output.xlsx
+++ b/kubernetes cmd/kubernetes_output.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>pod/flask-app-d9fbd54bd-m82dl</t>
+          <t>pod/flask-app-d9fbd54bd-272h4</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,14 +486,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>67s</t>
+          <t>92s</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>pod/flask-app-d9fbd54bd-rdjsd</t>
+          <t>pod/flask-app-d9fbd54bd-298qm</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -513,16 +513,2662 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>67s</t>
+          <t>94s</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-2cpxd</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ContainerCreating</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-4g57l</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-4lvnh</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-4spqj</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>14m</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-56ctg</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-58cl5</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-5jf97</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-5tjnl</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ContainerCreating</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-5z8wf</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-67vl6</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-6852k</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-6rnq2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ContainerCreating</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-74hbj</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-78pnd</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-7f2jh</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-992rx</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-9bzck</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-9cl4p</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ContainerCreating</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-9pttn</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-9q924</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-b79jc</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-bh7q6</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-bqbr9</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-btn7b</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-bwg6k</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ContainerCreating</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-c4f2q</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ContainerCreating</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-c95qf</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-cf2nv</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-cfb5w</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-czd48</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-dfvtv</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-f42m7</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-ggrt6</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-glrgp</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-grg7r</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-h66vv</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-hqz99</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-hrvdp</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>14m</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-hzh4k</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-jj9gs</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-jqslt</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-kc429</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-kcp25</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-l4tn9</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>ContainerCreating</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-lckk6</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-lcsnb</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-ldsfj</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-ljh5t</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-lkvdp</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-lsj8n</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-lxpvz</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-m925z</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-m9fvq</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-m9xb8</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-mlblp</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-mnm8h</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-mqngn</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-mvtj7</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-nhr6q</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-nkh97</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-nlqbr</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-nnslr</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>ContainerCreating</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-nrk87</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-p2h77</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-pdsmh</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-ph9vp</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-q5fgm</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-q88dt</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-qdc9c</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-qt468</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-r5htp</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-r9s7n</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-rdsxn</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-rvnwm</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-rw87k</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-s5fc8</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-sfn6k</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-sg4g4</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-sqvz8</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-tbnbj</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-tkrp2</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-tp9kp</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-ttqqx</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-tvwgz</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-vdc2s</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-vdqdj</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-vggt4</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-vghkh</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-vl8rg</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-vrcb5</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-wbvx2</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>95s</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-whslb</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-xghv7</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-xwjcs</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>0/1</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>ContainerCreating</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>91s</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-z4rlb</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-z58tm</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-z9ml9</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>94s</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>pod/flask-app-d9fbd54bd-zw6vr</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>1/1</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>93s</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -603,7 +3249,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>16h</t>
+          <t>3d</t>
         </is>
       </c>
     </row>
@@ -635,7 +3281,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>16h</t>
+          <t>3d1h</t>
         </is>
       </c>
     </row>
@@ -701,22 +3347,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>91/100</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>91</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>16h</t>
+          <t>3d</t>
         </is>
       </c>
     </row>
@@ -796,7 +3442,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>16h</t>
+          <t>3d</t>
         </is>
       </c>
     </row>
@@ -808,22 +3454,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>100</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>91</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>15h</t>
+          <t>2d23h</t>
         </is>
       </c>
     </row>

</xml_diff>